<commit_message>
now seed session data correctly
</commit_message>
<xml_diff>
--- a/database/seeds/_data/SessionsDate.xlsx
+++ b/database/seeds/_data/SessionsDate.xlsx
@@ -26,7 +26,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -60,7 +60,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -355,10 +355,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A7" activeCellId="5" sqref="A5:XFD5 A9:XFD10 A11:XFD12 A8:XFD8 A6:XFD6 A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -421,14 +421,6 @@
       <c r="D4" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>